<commit_message>
Fixed the gausian 5x5 blur GLSL code
</commit_message>
<xml_diff>
--- a/6023_Algor_Gems_(2025)/Projects-Tests/Project_1/6023 Gems_Project_1_W24_Marking_Scheme.xlsx
+++ b/6023_Algor_Gems_(2025)/Projects-Tests/Project_1/6023 Gems_Project_1_W24_Marking_Scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2024-2025\GDP202425\6023_Algor_Gems_(2025)\Projects-Tests\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021DBD85-8A52-4069-8733-9DACBDC69E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59254846-992B-425A-A23D-F37CCA79E956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Snotify" sheetId="1" r:id="rId1"/>
@@ -1535,75 +1535,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1616,6 +1547,75 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2114,263 +2114,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="131" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="26"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="26"/>
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="26"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="26"/>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="26"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="26"/>
       <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="26"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="26"/>
       <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
       <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
       <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
       <c r="B28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="26"/>
       <c r="B29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="26"/>
       <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="8"/>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="14" t="s">
         <v>1</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="8"/>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="39"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="14" t="s">
         <v>1</v>
       </c>
@@ -2392,190 +2392,190 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
-      <c r="B35" s="21" t="s">
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="22"/>
+      <c r="B35" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="17" t="str">
+      <c r="C35" s="33"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="35" t="str">
         <f>IF(ISNUMBER(C41+C36),((C41+C36)/100)*0.8,"-")</f>
         <v>-</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="38">
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.35">
+      <c r="A36" s="23"/>
       <c r="B36" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="27">
+      <c r="D36" s="42">
         <v>40</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="23"/>
       <c r="B37" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="23"/>
       <c r="B38" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="23"/>
       <c r="B39" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="31"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+    </row>
+    <row r="40" spans="1:6" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="23"/>
       <c r="B40" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+    </row>
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.35">
+      <c r="A41" s="23"/>
       <c r="B41" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="27">
+      <c r="D41" s="42">
         <v>60</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="23"/>
       <c r="B42" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="23"/>
       <c r="B43" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="23"/>
       <c r="B44" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:6" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+    </row>
+    <row r="45" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+      <c r="A45" s="23"/>
       <c r="B45" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="23"/>
       <c r="B46" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="23"/>
       <c r="B47" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="23"/>
       <c r="B48" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-    </row>
-    <row r="49" spans="1:6" ht="90.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+    </row>
+    <row r="49" spans="1:6" ht="93" x14ac:dyDescent="0.35">
+      <c r="A49" s="23"/>
       <c r="B49" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+    </row>
+    <row r="50" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="23"/>
       <c r="B50" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-    </row>
-    <row r="51" spans="1:6" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+    </row>
+    <row r="51" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="24"/>
       <c r="B51" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="41"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E52" s="16">
         <f>SUM(E33:E51)</f>
         <v>0</v>
@@ -2587,6 +2587,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E35:E51"/>
+    <mergeCell ref="F35:F51"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="C41:C51"/>
+    <mergeCell ref="D41:D51"/>
     <mergeCell ref="A35:A51"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="A19:A31"/>
@@ -2596,13 +2603,6 @@
     <mergeCell ref="D19:D31"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E35:E51"/>
-    <mergeCell ref="F35:F51"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="C41:C51"/>
-    <mergeCell ref="D41:D51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2614,375 +2614,375 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696ABFA2-1B44-41E5-8BA4-0C993B89F93C}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="131" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="42.85546875" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="26"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="26"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="26"/>
       <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="26"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="26"/>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="26"/>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" s="26"/>
       <c r="B21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="26"/>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="26"/>
       <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="26"/>
       <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="26"/>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="26"/>
       <c r="B26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
       <c r="B27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
       <c r="B28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="26"/>
       <c r="B29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="26"/>
       <c r="B30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="41" t="s">
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="23"/>
+      <c r="B33" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="45">
         <v>0.4</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="42" t="s">
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="23"/>
+      <c r="B34" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-    </row>
-    <row r="35" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
-      <c r="B35" s="42" t="s">
+      <c r="C34" s="40"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+    </row>
+    <row r="35" spans="1:6" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="23"/>
+      <c r="B35" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="41" t="s">
+      <c r="C35" s="40"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="23"/>
+      <c r="B36" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="45">
         <v>0.6</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="42" t="s">
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="23"/>
+      <c r="B37" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="43" t="s">
+      <c r="C37" s="40"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="23"/>
+      <c r="B38" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="42" t="s">
+      <c r="C38" s="40"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="23"/>
+      <c r="B39" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="42" t="s">
+      <c r="C39" s="40"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="23"/>
+      <c r="B40" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="42" t="s">
+      <c r="C40" s="40"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="23"/>
+      <c r="B41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="43" t="s">
+      <c r="C41" s="40"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+    </row>
+    <row r="42" spans="1:6" ht="93" x14ac:dyDescent="0.35">
+      <c r="A42" s="23"/>
+      <c r="B42" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="44" t="s">
+      <c r="C42" s="40"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+    </row>
+    <row r="43" spans="1:6" ht="78" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="24"/>
+      <c r="B43" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="41"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E44" s="16">
         <f>SUM(E33:E43)</f>
         <v>0</v>
@@ -2994,6 +2994,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="C5:C18"/>
+    <mergeCell ref="D5:D18"/>
+    <mergeCell ref="A19:A31"/>
+    <mergeCell ref="C19:C31"/>
+    <mergeCell ref="D19:D31"/>
     <mergeCell ref="A33:A43"/>
     <mergeCell ref="E33:E43"/>
     <mergeCell ref="F33:F43"/>
@@ -3001,12 +3007,6 @@
     <mergeCell ref="D33:D35"/>
     <mergeCell ref="C36:C43"/>
     <mergeCell ref="D36:D43"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="C5:C18"/>
-    <mergeCell ref="D5:D18"/>
-    <mergeCell ref="A19:A31"/>
-    <mergeCell ref="C19:C31"/>
-    <mergeCell ref="D19:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>